<commit_message>
cas neadditionalinfo in excel updated
</commit_message>
<xml_diff>
--- a/TelcobrightVS13/Projects/UtilInstallConfig/config/allDeployment/cas/_helper/casOperatorInfo.xlsx
+++ b/TelcobrightVS13/Projects/UtilInstallConfig/config/allDeployment/cas/_helper/casOperatorInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\allDeployment\cas\_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sftproot\TelcobrightProject\TelcobrightVS13\Projects\UtilInstallConfig\config\allDeployment\cas\_helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="342">
   <si>
     <t>operator</t>
   </si>
@@ -1031,6 +1031,24 @@
   </si>
   <si>
     <t>D:\telcobright\vault\resources\CDR\gazinetworks\tdmKhlBogra\Khulna</t>
+  </si>
+  <si>
+    <t>MargeProcessing</t>
+  </si>
+  <si>
+    <t>PreDecodeAsTextFile</t>
+  </si>
+  <si>
+    <t>MaxConcurrentFilesForParallelPreDecoding</t>
+  </si>
+  <si>
+    <t>MinRowCountToStartBatchCdrProcessing</t>
+  </si>
+  <si>
+    <t>MaxNumberOfFilesInPreDecodedDirectory</t>
+  </si>
+  <si>
+    <t>maxParallelFileForPreDecode</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1291,7 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1383,6 +1401,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1825,11 +1844,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X54"/>
+  <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD3" sqref="AD3:AD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1854,9 +1873,13 @@
     <col min="22" max="22" width="25.42578125" customWidth="1"/>
     <col min="23" max="23" width="31.7109375" customWidth="1"/>
     <col min="24" max="24" width="20" customWidth="1"/>
+    <col min="27" max="27" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15">
+    <row r="1" spans="1:30" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1929,8 +1952,26 @@
       <c r="X1" s="19" t="s">
         <v>22</v>
       </c>
+      <c r="Y1" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="Z1" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>341</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:30" ht="15.75" thickTop="1">
       <c r="A2" s="20" t="s">
         <v>23</v>
       </c>
@@ -2002,8 +2043,29 @@
       <c r="W2">
         <v>285</v>
       </c>
+      <c r="X2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>30</v>
+      </c>
+      <c r="AB2">
+        <v>70000</v>
+      </c>
+      <c r="AC2" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:30" ht="15">
       <c r="A3" s="20" t="s">
         <v>23</v>
       </c>
@@ -2076,8 +2138,29 @@
       <c r="W3">
         <v>286</v>
       </c>
+      <c r="X3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>30</v>
+      </c>
+      <c r="AB3">
+        <v>70000</v>
+      </c>
+      <c r="AC3">
+        <v>500</v>
+      </c>
+      <c r="AD3" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:30" ht="15">
       <c r="A4" s="20" t="s">
         <v>39</v>
       </c>
@@ -2149,8 +2232,29 @@
       <c r="W4">
         <v>287</v>
       </c>
+      <c r="X4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB4" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC4" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD4" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:30" ht="15">
       <c r="A5" s="20" t="s">
         <v>39</v>
       </c>
@@ -2218,8 +2322,29 @@
       <c r="W5">
         <v>288</v>
       </c>
+      <c r="X5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y5" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB5" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC5" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD5" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:30" ht="15">
       <c r="A6" s="20" t="s">
         <v>52</v>
       </c>
@@ -2292,8 +2417,29 @@
       <c r="W6">
         <v>289</v>
       </c>
+      <c r="X6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB6" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC6" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD6" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:30" ht="15">
       <c r="A7" s="20" t="s">
         <v>52</v>
       </c>
@@ -2366,8 +2512,29 @@
       <c r="W7">
         <v>290</v>
       </c>
+      <c r="X7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y7" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB7" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC7" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD7" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" s="14" customFormat="1" ht="14.25">
+    <row r="8" spans="1:30" s="14" customFormat="1" ht="15">
       <c r="A8" s="14" t="s">
         <v>65</v>
       </c>
@@ -2439,8 +2606,29 @@
       <c r="W8">
         <v>291</v>
       </c>
+      <c r="X8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y8" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB8" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC8" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD8" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="15">
+    <row r="9" spans="1:30" ht="15">
       <c r="A9" s="20" t="s">
         <v>65</v>
       </c>
@@ -2513,8 +2701,29 @@
       <c r="W9">
         <v>292</v>
       </c>
+      <c r="X9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y9" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB9" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC9" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD9" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" ht="15">
+    <row r="10" spans="1:30" ht="15">
       <c r="A10" s="24" t="s">
         <v>76</v>
       </c>
@@ -2582,8 +2791,29 @@
       <c r="W10">
         <v>293</v>
       </c>
+      <c r="X10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y10" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB10" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC10" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD10" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" ht="15">
+    <row r="11" spans="1:30" ht="15">
       <c r="A11" s="24" t="s">
         <v>76</v>
       </c>
@@ -2652,8 +2882,29 @@
       <c r="W11">
         <v>294</v>
       </c>
+      <c r="X11" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y11" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB11" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC11" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD11" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" ht="15">
+    <row r="12" spans="1:30" ht="15">
       <c r="A12" s="20" t="s">
         <v>76</v>
       </c>
@@ -2724,8 +2975,29 @@
       <c r="W12">
         <v>295</v>
       </c>
+      <c r="X12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y12" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB12" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC12" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD12" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" s="15" customFormat="1" ht="15">
+    <row r="13" spans="1:30" s="15" customFormat="1" ht="15">
       <c r="A13" s="28" t="s">
         <v>93</v>
       </c>
@@ -2797,8 +3069,29 @@
       <c r="W13">
         <v>296</v>
       </c>
+      <c r="X13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y13" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB13" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC13" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD13" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" ht="15">
+    <row r="14" spans="1:30" ht="15">
       <c r="A14" s="20" t="s">
         <v>93</v>
       </c>
@@ -2871,8 +3164,29 @@
       <c r="W14">
         <v>297</v>
       </c>
+      <c r="X14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y14" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB14" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC14" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD14" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" ht="15">
+    <row r="15" spans="1:30" ht="15">
       <c r="A15" s="20" t="s">
         <v>93</v>
       </c>
@@ -2945,8 +3259,29 @@
       <c r="W15">
         <v>298</v>
       </c>
+      <c r="X15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y15" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB15" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC15" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD15" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" ht="15">
+    <row r="16" spans="1:30" ht="15">
       <c r="A16" s="20" t="s">
         <v>110</v>
       </c>
@@ -3018,8 +3353,29 @@
       <c r="W16">
         <v>299</v>
       </c>
+      <c r="X16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y16" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB16" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC16" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD16" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" ht="15">
+    <row r="17" spans="1:30" ht="15">
       <c r="A17" s="20" t="s">
         <v>110</v>
       </c>
@@ -3087,8 +3443,29 @@
       <c r="W17">
         <v>300</v>
       </c>
+      <c r="X17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y17" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB17" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC17" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD17" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" s="38" customFormat="1" ht="14.25">
+    <row r="18" spans="1:30" s="38" customFormat="1" ht="15">
       <c r="A18" s="38" t="s">
         <v>110</v>
       </c>
@@ -3158,8 +3535,29 @@
       <c r="W18" s="38">
         <v>301</v>
       </c>
+      <c r="X18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y18" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB18" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC18" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD18" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" s="38" customFormat="1" ht="14.25">
+    <row r="19" spans="1:30" s="38" customFormat="1" ht="15">
       <c r="A19" s="38" t="s">
         <v>110</v>
       </c>
@@ -3229,8 +3627,29 @@
       <c r="W19" s="38">
         <v>301</v>
       </c>
+      <c r="X19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y19" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB19" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC19" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD19" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" ht="15">
+    <row r="20" spans="1:30" ht="15">
       <c r="A20" s="20" t="s">
         <v>127</v>
       </c>
@@ -3303,8 +3722,29 @@
       <c r="W20">
         <v>302</v>
       </c>
+      <c r="X20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y20" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB20" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC20" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD20" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" ht="15">
+    <row r="21" spans="1:30" ht="15">
       <c r="A21" s="20" t="s">
         <v>127</v>
       </c>
@@ -3377,8 +3817,29 @@
       <c r="W21">
         <v>303</v>
       </c>
+      <c r="X21" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y21" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB21" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC21" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD21" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" ht="15">
+    <row r="22" spans="1:30" ht="15">
       <c r="A22" s="20" t="s">
         <v>138</v>
       </c>
@@ -3451,8 +3912,29 @@
       <c r="W22">
         <v>304</v>
       </c>
+      <c r="X22" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y22" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB22" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC22" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD22" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" ht="15">
+    <row r="23" spans="1:30" ht="15">
       <c r="A23" s="20" t="s">
         <v>138</v>
       </c>
@@ -3524,8 +4006,29 @@
       <c r="W23">
         <v>305</v>
       </c>
+      <c r="X23" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y23" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB23" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC23" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD23" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" s="16" customFormat="1" ht="15">
+    <row r="24" spans="1:30" s="16" customFormat="1" ht="15">
       <c r="A24" s="20" t="s">
         <v>150</v>
       </c>
@@ -3597,8 +4100,29 @@
       <c r="W24">
         <v>306</v>
       </c>
+      <c r="X24" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y24" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB24" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC24" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD24" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" s="16" customFormat="1" ht="15">
+    <row r="25" spans="1:30" s="16" customFormat="1" ht="15">
       <c r="A25" s="20" t="s">
         <v>150</v>
       </c>
@@ -3671,8 +4195,29 @@
       <c r="W25">
         <v>307</v>
       </c>
+      <c r="X25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y25" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB25" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC25" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD25" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" ht="15">
+    <row r="26" spans="1:30" ht="15">
       <c r="A26" s="20" t="s">
         <v>161</v>
       </c>
@@ -3745,8 +4290,29 @@
       <c r="W26">
         <v>308</v>
       </c>
+      <c r="X26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y26" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB26" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC26" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD26" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" ht="15">
+    <row r="27" spans="1:30" ht="15">
       <c r="A27" s="20" t="s">
         <v>161</v>
       </c>
@@ -3819,8 +4385,29 @@
       <c r="W27">
         <v>309</v>
       </c>
+      <c r="X27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y27" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB27" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC27" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD27" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" s="17" customFormat="1" ht="14.25">
+    <row r="28" spans="1:30" s="17" customFormat="1" ht="15">
       <c r="A28" s="17" t="s">
         <v>171</v>
       </c>
@@ -3892,8 +4479,29 @@
       <c r="W28">
         <v>310</v>
       </c>
+      <c r="X28" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y28" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB28" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC28" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD28" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="29" spans="1:23" ht="15">
+    <row r="29" spans="1:30" ht="15">
       <c r="A29" s="20" t="s">
         <v>171</v>
       </c>
@@ -3964,8 +4572,29 @@
       <c r="W29">
         <v>311</v>
       </c>
+      <c r="X29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y29" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB29" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC29" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD29" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="30" spans="1:23" ht="15">
+    <row r="30" spans="1:30" ht="15">
       <c r="A30" s="20" t="s">
         <v>181</v>
       </c>
@@ -4038,8 +4667,29 @@
       <c r="W30">
         <v>312</v>
       </c>
+      <c r="X30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y30" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB30" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC30" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD30" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="31" spans="1:23" ht="15">
+    <row r="31" spans="1:30" ht="15">
       <c r="A31" s="20" t="s">
         <v>181</v>
       </c>
@@ -4110,8 +4760,29 @@
       <c r="W31">
         <v>313</v>
       </c>
+      <c r="X31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y31" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB31" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC31" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD31" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="32" spans="1:23" s="17" customFormat="1" ht="14.25">
+    <row r="32" spans="1:30" s="17" customFormat="1" ht="15">
       <c r="A32" s="17" t="s">
         <v>193</v>
       </c>
@@ -4183,8 +4854,29 @@
       <c r="W32">
         <v>314</v>
       </c>
+      <c r="X32" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y32" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB32" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC32" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD32" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="33" spans="1:23" ht="15">
+    <row r="33" spans="1:30" ht="15">
       <c r="A33" s="20" t="s">
         <v>193</v>
       </c>
@@ -4255,8 +4947,29 @@
       <c r="W33">
         <v>315</v>
       </c>
+      <c r="X33" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y33" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB33" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC33" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD33" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="34" spans="1:23" ht="15">
+    <row r="34" spans="1:30" ht="15">
       <c r="A34" s="20" t="s">
         <v>204</v>
       </c>
@@ -4329,8 +5042,29 @@
       <c r="W34">
         <v>316</v>
       </c>
+      <c r="X34" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y34" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB34" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC34" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD34" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="35" spans="1:23" ht="15">
+    <row r="35" spans="1:30" ht="15">
       <c r="A35" s="20" t="s">
         <v>204</v>
       </c>
@@ -4402,8 +5136,29 @@
       <c r="W35">
         <v>317</v>
       </c>
+      <c r="X35" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y35" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB35" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC35" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD35" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="36" spans="1:23" ht="15">
+    <row r="36" spans="1:30" ht="15">
       <c r="A36" s="20" t="s">
         <v>215</v>
       </c>
@@ -4475,8 +5230,29 @@
       <c r="W36">
         <v>318</v>
       </c>
+      <c r="X36" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y36" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB36" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC36" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD36" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="37" spans="1:23" ht="15">
+    <row r="37" spans="1:30" ht="15">
       <c r="A37" s="20" t="s">
         <v>215</v>
       </c>
@@ -4548,8 +5324,29 @@
       <c r="W37">
         <v>319</v>
       </c>
+      <c r="X37" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y37" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA37" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB37" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC37" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD37" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="38" spans="1:23" ht="15">
+    <row r="38" spans="1:30" ht="15">
       <c r="A38" s="20" t="s">
         <v>226</v>
       </c>
@@ -4619,8 +5416,29 @@
       <c r="W38">
         <v>320</v>
       </c>
+      <c r="X38" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y38" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB38" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC38" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD38" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="39" spans="1:23" ht="15">
+    <row r="39" spans="1:30" ht="15">
       <c r="A39" s="20" t="s">
         <v>226</v>
       </c>
@@ -4692,8 +5510,29 @@
       <c r="W39">
         <v>321</v>
       </c>
+      <c r="X39" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y39" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB39" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC39" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD39" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="40" spans="1:23" ht="15">
+    <row r="40" spans="1:30" ht="15">
       <c r="A40" s="20" t="s">
         <v>240</v>
       </c>
@@ -4766,8 +5605,29 @@
       <c r="W40">
         <v>322</v>
       </c>
+      <c r="X40" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y40" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB40" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC40" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD40" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="41" spans="1:23" ht="15">
+    <row r="41" spans="1:30" ht="15">
       <c r="A41" s="20" t="s">
         <v>240</v>
       </c>
@@ -4839,8 +5699,29 @@
       <c r="W41">
         <v>323</v>
       </c>
+      <c r="X41" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y41" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB41" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC41" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD41" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="42" spans="1:23" ht="15">
+    <row r="42" spans="1:30" ht="15">
       <c r="A42" s="20" t="s">
         <v>251</v>
       </c>
@@ -4912,8 +5793,29 @@
       <c r="W42">
         <v>324</v>
       </c>
+      <c r="X42" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y42" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB42" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC42" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD42" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="43" spans="1:23" ht="15">
+    <row r="43" spans="1:30" ht="15">
       <c r="A43" s="20" t="s">
         <v>251</v>
       </c>
@@ -4986,8 +5888,29 @@
       <c r="W43">
         <v>325</v>
       </c>
+      <c r="X43" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y43" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA43" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB43" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC43" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD43" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="44" spans="1:23" ht="15">
+    <row r="44" spans="1:30" ht="15">
       <c r="A44" s="20" t="s">
         <v>260</v>
       </c>
@@ -5060,8 +5983,29 @@
       <c r="W44">
         <v>326</v>
       </c>
+      <c r="X44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y44" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z44" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA44" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB44" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC44" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD44" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="45" spans="1:23" ht="15">
+    <row r="45" spans="1:30" ht="15">
       <c r="A45" s="20" t="s">
         <v>260</v>
       </c>
@@ -5133,8 +6077,29 @@
       <c r="W45">
         <v>327</v>
       </c>
+      <c r="X45" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y45" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB45" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC45" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD45" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="46" spans="1:23" ht="15">
+    <row r="46" spans="1:30" ht="15">
       <c r="A46" s="20" t="s">
         <v>271</v>
       </c>
@@ -5207,8 +6172,29 @@
       <c r="W46">
         <v>328</v>
       </c>
+      <c r="X46" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y46" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB46" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC46" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD46" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="47" spans="1:23" ht="15">
+    <row r="47" spans="1:30" ht="15">
       <c r="A47" s="20" t="s">
         <v>271</v>
       </c>
@@ -5281,8 +6267,29 @@
       <c r="W47">
         <v>329</v>
       </c>
+      <c r="X47" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y47" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA47" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB47" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC47" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD47" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="48" spans="1:23" s="14" customFormat="1" ht="14.25">
+    <row r="48" spans="1:30" s="14" customFormat="1" ht="15">
       <c r="A48" s="14" t="s">
         <v>281</v>
       </c>
@@ -5354,8 +6361,29 @@
       <c r="W48">
         <v>330</v>
       </c>
+      <c r="X48" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y48" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z48" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA48" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB48" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC48" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD48" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="49" spans="1:23" ht="15">
+    <row r="49" spans="1:30" ht="15">
       <c r="A49" s="20" t="s">
         <v>281</v>
       </c>
@@ -5428,8 +6456,29 @@
       <c r="W49">
         <v>331</v>
       </c>
+      <c r="X49" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y49" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA49" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB49" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC49" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD49" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="50" spans="1:23" ht="15">
+    <row r="50" spans="1:30" ht="15">
       <c r="A50" s="20" t="s">
         <v>281</v>
       </c>
@@ -5502,8 +6551,29 @@
       <c r="W50">
         <v>332</v>
       </c>
+      <c r="X50" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y50" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA50" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB50" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC50" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD50" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="51" spans="1:23" s="18" customFormat="1" ht="14.25">
+    <row r="51" spans="1:30" s="18" customFormat="1" ht="15">
       <c r="A51" s="18" t="s">
         <v>296</v>
       </c>
@@ -5571,8 +6641,29 @@
       <c r="W51">
         <v>333</v>
       </c>
+      <c r="X51" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y51" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z51" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA51" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB51" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC51" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD51" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="52" spans="1:23" ht="15">
+    <row r="52" spans="1:30" ht="15">
       <c r="A52" s="20" t="s">
         <v>296</v>
       </c>
@@ -5644,8 +6735,29 @@
       <c r="W52">
         <v>334</v>
       </c>
+      <c r="X52" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y52" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA52" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB52" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC52" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD52" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="53" spans="1:23" ht="15">
+    <row r="53" spans="1:30" ht="15">
       <c r="A53" s="20" t="s">
         <v>308</v>
       </c>
@@ -5717,8 +6829,29 @@
       <c r="W53">
         <v>335</v>
       </c>
+      <c r="X53" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y53" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z53" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA53" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB53" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC53" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD53" s="51">
+        <v>10</v>
+      </c>
     </row>
-    <row r="54" spans="1:23" ht="15">
+    <row r="54" spans="1:30" ht="15">
       <c r="A54" s="20" t="s">
         <v>308</v>
       </c>
@@ -5789,6 +6922,27 @@
       </c>
       <c r="W54">
         <v>336</v>
+      </c>
+      <c r="X54" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y54" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z54" s="51">
+        <v>1</v>
+      </c>
+      <c r="AA54" s="51">
+        <v>30</v>
+      </c>
+      <c r="AB54" s="51">
+        <v>70000</v>
+      </c>
+      <c r="AC54" s="51">
+        <v>500</v>
+      </c>
+      <c r="AD54" s="51">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6177,27 +7331,27 @@
     <row r="23" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="24" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="25" spans="2:9" ht="12.75" customHeight="1">
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="2:9" ht="12.75" customHeight="1">
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="2:9" ht="12.75" customHeight="1">
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
     </row>
     <row r="28" spans="2:9" ht="12.75" customHeight="1"/>
     <row r="29" spans="2:9" ht="12.75" customHeight="1"/>

</xml_diff>